<commit_message>
sales3.xlss -> salex4.xlss -> umjesto numericki napravio sam kategorije po kvartilama q1, q2, q3
</commit_message>
<xml_diff>
--- a/DecisionTree-1/Files/play1.xlsx
+++ b/DecisionTree-1/Files/play1.xlsx
@@ -8,19 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_ML\DecisionTree-1\DecisionTree-1\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2EDF3C-0200-4D79-B23D-CDAFBBDE2D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D917646-71F9-45A2-8CEE-3369CB4AD342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="podaci" sheetId="1" r:id="rId1"/>
+    <sheet name="gini index outlook" sheetId="2" r:id="rId2"/>
+    <sheet name="gini index windy" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'gini index outlook'!$A$1:$B$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'gini index windy'!$A$1:$B$16</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="16">
   <si>
     <t>Outlook</t>
   </si>
@@ -44,13 +63,114 @@
   </si>
   <si>
     <t>Don't Play</t>
+  </si>
+  <si>
+    <t>udio u skupu</t>
+  </si>
+  <si>
+    <t>score play</t>
+  </si>
+  <si>
+    <t>score not play</t>
+  </si>
+  <si>
+    <t>nečistoća</t>
+  </si>
+  <si>
+    <t>Doprinos Gini-u</t>
+  </si>
+  <si>
+    <t>score ukupno</t>
+  </si>
+  <si>
+    <r>
+      <t>Windy=FALSE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> → gotovo svi </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Play</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (8 Play, 1 Don't Play) → skoro čist skup</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Windy=TRUE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> → većina </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Don't Play</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> → dovoljno čisto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> da ovo bude _____________</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +181,20 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -102,12 +236,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,230 +582,915 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>65</v>
       </c>
-      <c r="C2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>70</v>
       </c>
-      <c r="C3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>68</v>
       </c>
-      <c r="C4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>72</v>
       </c>
-      <c r="C5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>75</v>
       </c>
-      <c r="C6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>80</v>
       </c>
-      <c r="C7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>70</v>
       </c>
-      <c r="C8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>68</v>
       </c>
-      <c r="C9" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>75</v>
       </c>
-      <c r="C10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>90</v>
       </c>
-      <c r="C11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>75</v>
       </c>
-      <c r="C12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>78</v>
       </c>
-      <c r="C13" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>65</v>
       </c>
-      <c r="C14" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>70</v>
       </c>
-      <c r="C15" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>60</v>
       </c>
-      <c r="C16" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E615F81C-A9CE-4743-B210-53CB98952D60}">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3">
+        <v>3</v>
+      </c>
+      <c r="D23" s="4">
+        <f>SUM(B23:C23)</f>
+        <v>6</v>
+      </c>
+      <c r="F23" s="6">
+        <f>B23/$D23</f>
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="6">
+        <f>C23/$D23</f>
+        <v>0.5</v>
+      </c>
+      <c r="H23" s="8">
+        <f>F23*F23+G23*G23</f>
+        <v>0.5</v>
+      </c>
+      <c r="I23" s="8">
+        <f>1-H23</f>
+        <v>0.5</v>
+      </c>
+      <c r="J23" s="6">
+        <f>D23/D$26</f>
+        <v>0.4</v>
+      </c>
+      <c r="K23" s="6">
+        <f>I23*J23</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="3">
+        <v>3</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" ref="D24:D25" si="0">SUM(B24:C24)</f>
+        <v>4</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" ref="F24:F25" si="1">B24/$D24</f>
+        <v>0.75</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" ref="G24:G25" si="2">C24/$D24</f>
+        <v>0.25</v>
+      </c>
+      <c r="H24" s="8">
+        <f t="shared" ref="H24:H25" si="3">F24*F24+G24*G24</f>
+        <v>0.625</v>
+      </c>
+      <c r="I24" s="8">
+        <f t="shared" ref="I24:I25" si="4">1-H24</f>
+        <v>0.375</v>
+      </c>
+      <c r="J24" s="6">
+        <f>D24/D$26</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" ref="K24:K25" si="5">I24*J24</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="3">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3">
+        <v>3</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F25" s="6">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="H25" s="8">
+        <f t="shared" si="3"/>
+        <v>0.52</v>
+      </c>
+      <c r="I25" s="8">
+        <f t="shared" si="4"/>
+        <v>0.48</v>
+      </c>
+      <c r="J25" s="6">
+        <f>D25/D$26</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K25" s="6">
+        <f t="shared" si="5"/>
+        <v>0.15999999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <f>SUM(B23:B25)</f>
+        <v>8</v>
+      </c>
+      <c r="C26" s="4">
+        <f>SUM(C23:C25)</f>
+        <v>7</v>
+      </c>
+      <c r="D26" s="4">
+        <f>SUM(D23:D25)</f>
+        <v>15</v>
+      </c>
+      <c r="K26" s="9">
+        <f>SUM(K23:K25)</f>
+        <v>0.46</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B16" xr:uid="{E615F81C-A9CE-4743-B210-53CB98952D60}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223345C6-0FA6-43B2-8529-92215F0537E0}">
+  <dimension ref="A1:K31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="G3" s="3">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3">
+        <v>3</v>
+      </c>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3</v>
+      </c>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="b">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="b">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="b">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="b">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="b">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B23" s="3">
+        <v>8</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4">
+        <f>SUM(B23:C23)</f>
+        <v>9</v>
+      </c>
+      <c r="F23" s="6">
+        <f>B23/$D23</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="G23" s="6">
+        <f>C23/$D23</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="H23" s="8">
+        <f>F23*F23+G23*G23</f>
+        <v>0.80246913580246915</v>
+      </c>
+      <c r="I23" s="8">
+        <f>1-H23</f>
+        <v>0.19753086419753085</v>
+      </c>
+      <c r="J23" s="6">
+        <f>D23/D$25</f>
+        <v>0.6</v>
+      </c>
+      <c r="K23" s="6">
+        <f>I23*J23</f>
+        <v>0.11851851851851851</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3">
+        <v>5</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" ref="D24" si="0">SUM(B24:C24)</f>
+        <v>6</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" ref="F24:G24" si="1">B24/$D24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="1"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H24" s="8">
+        <f t="shared" ref="H24" si="2">F24*F24+G24*G24</f>
+        <v>0.72222222222222232</v>
+      </c>
+      <c r="I24" s="8">
+        <f t="shared" ref="I24" si="3">1-H24</f>
+        <v>0.27777777777777768</v>
+      </c>
+      <c r="J24" s="6">
+        <f>D24/D$25</f>
+        <v>0.4</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" ref="K24" si="4">I24*J24</f>
+        <v>0.11111111111111108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <f>SUM(B23:B24)</f>
+        <v>9</v>
+      </c>
+      <c r="C25" s="4">
+        <f>SUM(C23:C24)</f>
+        <v>6</v>
+      </c>
+      <c r="D25" s="4">
+        <f>SUM(D23:D24)</f>
+        <v>15</v>
+      </c>
+      <c r="K25" s="9">
+        <f>SUM(K23:K24)</f>
+        <v>0.22962962962962957</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B16" xr:uid="{223345C6-0FA6-43B2-8529-92215F0537E0}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>